<commit_message>
some changes in main.m
</commit_message>
<xml_diff>
--- a/macro_factor/indicators/inputs/otr_30y.xlsx
+++ b/macro_factor/indicators/inputs/otr_30y.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>020005.IB</t>
   </si>
@@ -120,9 +120,6 @@
   </si>
   <si>
     <t>200004.IB</t>
-  </si>
-  <si>
-    <t>9802.IB</t>
   </si>
   <si>
     <t>200012.IB</t>
@@ -456,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A34"/>
+  <dimension ref="A1:A33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -629,11 +626,6 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A34" t="s">
-        <v>33</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>